<commit_message>
added updated Dashboard from Thomas
</commit_message>
<xml_diff>
--- a/Tools&Utilities/dashboards/OSS_SLU_CICD_Dashboard.xlsx
+++ b/Tools&Utilities/dashboards/OSS_SLU_CICD_Dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinduong/oss_cicd_automation/Tools&amp;Utilities/dashboards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danyu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF78458-35FD-B14E-9EE5-D2A17EABDBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26421DD2-F261-41FA-A3F7-865E5CF6B685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSS_SLU_CICD_Dashboard" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="115">
   <si>
     <t>Project_Name</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Custom CI/CD</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Requesting Help</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
   </si>
   <si>
     <t>CivicKit</t>
-  </si>
-  <si>
-    <t>Requesting Help (In Progress)</t>
   </si>
   <si>
     <t xml:space="preserve">Yes </t>
@@ -379,6 +373,12 @@
   </si>
   <si>
     <t>Avg issues completed:</t>
+  </si>
+  <si>
+    <t>Audit completed, gave suggestions on where to start for implentation of new CI/CD elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requested Help </t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -501,6 +501,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -807,27 +810,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="62.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -850,520 +853,523 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>35</v>
+        <v>114</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>113</v>
       </c>
       <c r="K3" s="1">
-        <v>46052</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>46064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1">
         <v>45964</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K5" s="1">
         <v>45974</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K7" s="1">
         <v>45993</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K8" s="1">
         <v>45924</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K17" s="1">
         <v>45993</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1375,117 +1381,117 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K19" s="1">
         <v>46062</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K21" s="1">
         <v>45975</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K22" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1494,50 +1500,50 @@
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K23" s="1">
         <v>45993</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K24" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1549,148 +1555,148 @@
         <v>10</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K25" s="1">
         <v>45943</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K26" s="1">
         <v>45969</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K27" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K28" s="1">
         <v>46057</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1">
-        <v>46053</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>46064</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
         <v>47</v>
-      </c>
-      <c r="B37" t="s">
-        <v>49</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1699,178 +1705,178 @@
         <v>46057</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F43" s="14">
         <f>9/27</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F44" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F45">
         <f>1/2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" s="3" t="s">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B54" s="5"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="5"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated dashboard for BAIO request CI/CD help
</commit_message>
<xml_diff>
--- a/Tools&Utilities/dashboards/OSS_SLU_CICD_Dashboard.xlsx
+++ b/Tools&Utilities/dashboards/OSS_SLU_CICD_Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danyu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26421DD2-F261-41FA-A3F7-865E5CF6B685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCACDC13-729A-4107-8C53-3258B39B4603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2235" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OSS_SLU_CICD_Dashboard" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +461,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -476,7 +482,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -504,6 +510,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -810,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +873,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -879,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>33</v>
@@ -1146,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
@@ -1884,13 +1891,13 @@
     <sortCondition ref="A2:A28"/>
   </sortState>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C3 E6:G6 E16:G16 D2:E2 E9:G10 F11:G15 E18:G20 F22:G22 F27:G28 F24:G24 D4:D28 C5:C28 C36:D989" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C3 E6:G6 E16:G16 E11 E9:G10 F11:G15 E18:G20 F22:G22 F27:G28 F24:G24 D4:D28 C5:C28 C36:D989 D2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="F26 F7:F8 F17 F21 F4:F5 F29:F989" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"Custom CI/CD,Existing CI/CD,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E4:E5 E7:E8 E11:E15 E17 E21:E28 E35:E989" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="E4:E5 E7:E8 E35:E989 E17 E21:E28 E12:E15" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Not Checked,Audited,Requesting Help,Postponed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="G7:G8 G17 G25 H4:H24 H26:H989 G29:G989" xr:uid="{00000000-0002-0000-0000-000004000000}">

</xml_diff>